<commit_message>
Automatische test-sync: 2025-08-06 19:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,8 +738,63 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Zou jij dit even op kunnen pakken?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Zou jij dit even op kunnen pakken?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw bericht. Kunt u specifieker zijn over welke kwestie u wenst dat we oppakken? Graag ontvangen we meer details om u verder te kunnen helpen.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:27:43</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -759,7 +814,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -767,17 +822,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -819,7 +874,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,8 +793,60 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Zou jij dit even op kunnen pakken?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Zou jij dit even op kunnen pakken?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:29:59</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -814,7 +866,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +874,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -874,7 +926,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,8 +845,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun je dit voor me fixen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun je dit voor me fixen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:36:15</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -866,7 +918,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -874,17 +926,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -926,7 +978,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -897,8 +897,60 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Los jij dit even af?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Los jij dit even af?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar planning@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:40:29</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -918,7 +970,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -926,17 +978,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -978,7 +1030,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -949,8 +949,63 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #1: Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw e-mail. We willen u graag informeren dat wij geen bestelling hebben ontvangen voor 100 M5-bouten. Mocht dit een vergissing zijn, dan kunt u uw bestelling plaatsen via onze website of ons telefonisch bereiken.
+Met vriendelijke groet,
+[Naam Bedrijf]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:44:13</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -970,7 +1025,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -978,17 +1033,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1003,7 +1058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1033,6 +1088,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1004,8 +1004,63 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #1: Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank je wel voor je bericht. Als je 100 M5-bouten wilt bestellen, kun je dit doen door naar onze website te gaan en het gewenste aantal toe te voegen aan je winkelwagen. Als je hulp nodig hebt bij het plaatsen van de bestelling, laat het ons dan weten en we helpen je graag verder.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:46:25</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1025,7 +1080,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1033,17 +1088,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1095,7 +1150,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1059,8 +1059,60 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #1: Bestel je 100 M5-bouten zodra je kan?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:48:14</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1080,7 +1132,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1088,17 +1140,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1150,7 +1202,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,8 +1111,60 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kun jij deze klant even bellen vandaag?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #1: Kun jij deze klant even bellen vandaag?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:51:40</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1132,7 +1184,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1140,17 +1192,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1165,7 +1217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1205,6 +1257,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 19:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1163,8 +1163,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Staan er nog EcoPro-700 op voorraad?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #1: Staan er nog EcoPro-700 op voorraad?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-06 19:54:49</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1184,7 +1236,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1192,17 +1244,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1254,7 +1306,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1215,8 +1215,60 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Is dit artikel momenteel beschikbaar?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #1: Is dit artikel momenteel beschikbaar?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:01:12</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1236,7 +1288,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1244,17 +1296,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1306,7 +1358,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1267,8 +1267,60 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Check jij even of dit nog geleverd kan worden?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #1: Check jij even of dit nog geleverd kan worden?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar inkoop@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:04:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1288,7 +1340,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1296,17 +1348,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1344,17 +1396,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,8 +1319,60 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Hebben jullie toevallig al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #1: Hebben jullie toevallig al iets gehoord?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Klantenservice / Contact</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:06:49</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1340,7 +1392,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1348,17 +1400,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1420,7 +1472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1371,8 +1371,60 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Laat maar weten of er nieuws is</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #1: Laat maar weten of er nieuws is</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Klantenservice / Opvolging</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:17:47</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1392,7 +1444,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1400,17 +1452,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1425,7 +1477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1475,6 +1527,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Klantenservice / Opvolging</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,8 +1423,60 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Laat maar weten of er nieuws is</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #1: Laat maar weten of er nieuws is</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Klantenservice / Opvolging</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar klantenservice@bedrijf.nl.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:21:18</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1444,7 +1496,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1452,17 +1504,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1534,7 +1586,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1475,8 +1475,64 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #1: Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Om je retour te kunnen bekijken, hebben we wat meer informatie nodig. Zou je ons je bestelnummer kunnen doorgeven, zodat we de status van je retour kunnen controleren?
+Alvast bedankt voor je medewerking.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:33:19</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1496,7 +1552,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1504,17 +1560,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1529,7 +1585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1589,6 +1645,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1531,8 +1531,63 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #1: Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Om je vraag over de status van je retour te kunnen beantwoorden, heb ik wat meer informatie nodig. Zou je alsjeblieft je ordernummer of traceernummer van de retourzending kunnen doorgeven? Dan kan ik dit voor je nakijken en je zo goed mogelijk helpen.
+Met vriendelijke groet,
+[Naam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:35:19</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1552,7 +1607,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1560,17 +1615,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1652,7 +1707,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-06 20:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-06.xlsx
+++ b/logs/mail_log_2025-08-06.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1586,8 +1586,64 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #1: Weten jullie al iets over mijn retour?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Om je vraag over je retour te beantwoorden, heb ik wat meer informatie nodig. Zou je ons je ordernummer of het track &amp; trace-nummer van de retourzending kunnen doorgeven? Op die manier kunnen we de status controleren en je verder helpen.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-08-06 20:39:04</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1607,7 +1663,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1615,17 +1671,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1683,17 +1739,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klantenservice / Contact</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klantenservice / Opvolging</t>
+          <t>Klantenservice / Contact</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1703,7 +1759,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Klantenservice / Opvolging</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>